<commit_message>
Message décrivant les modifications
</commit_message>
<xml_diff>
--- a/exports/All_Reclamations_Report.xlsx
+++ b/exports/All_Reclamations_Report.xlsx
@@ -11,12 +11,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
-  <si>
-    <t>N° de réclamation</t>
-  </si>
-  <si>
-    <t>BLN°</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+  <si>
+    <t>Bon Livraison</t>
+  </si>
+  <si>
+    <t>Wilaya</t>
   </si>
   <si>
     <t>Date De reclamation</t>
@@ -31,16 +31,7 @@
     <t>Télephone</t>
   </si>
   <si>
-    <t>Réclamant</t>
-  </si>
-  <si>
-    <t>Téléphone</t>
-  </si>
-  <si>
-    <t>Modalité de réception</t>
-  </si>
-  <si>
-    <t>Cause de retour</t>
+    <t>Probleme</t>
   </si>
   <si>
     <t>Informations Articles</t>
@@ -55,6 +46,9 @@
     <t>Quantité</t>
   </si>
   <si>
+    <t>Valeur</t>
+  </si>
+  <si>
     <t>État</t>
   </si>
   <si>
@@ -64,28 +58,22 @@
     <t>Pièces</t>
   </si>
   <si>
-    <t>25555555555</t>
-  </si>
-  <si>
-    <t>2024-08-06</t>
-  </si>
-  <si>
-    <t>2024-08-13</t>
-  </si>
-  <si>
-    <t>LAIB  FATEH</t>
-  </si>
-  <si>
-    <t>05456454</t>
-  </si>
-  <si>
-    <t>riad</t>
-  </si>
-  <si>
-    <t>0635659656</t>
-  </si>
-  <si>
-    <t>email</t>
+    <t>7257845278</t>
+  </si>
+  <si>
+    <t>Alger</t>
+  </si>
+  <si>
+    <t>12/08/2024</t>
+  </si>
+  <si>
+    <t>01/08/2024</t>
+  </si>
+  <si>
+    <t>LAIB  HAMID</t>
+  </si>
+  <si>
+    <t>0635515554</t>
   </si>
   <si>
     <t>erreurLivraison</t>
@@ -97,10 +85,13 @@
     <t>INTERRUPTEUR SIMPLE ALLUMAGE</t>
   </si>
   <si>
+    <t>25</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
-    <t>44</t>
+    <t>11000.DA</t>
   </si>
   <si>
     <t>En plus</t>
@@ -163,15 +154,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -517,13 +511,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O4"/>
+  <dimension ref="A1:N4"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
-    <col min="1" max="15" width="30" customWidth="1"/>
+    <col min="1" max="14" width="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -548,21 +542,14 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
+      <c r="N1" s="2"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -570,24 +557,24 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1" t="s">
+      <c r="H2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2" t="s">
-        <v>14</v>
-      </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -597,68 +584,61 @@
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
+      <c r="J3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="L3" s="1"/>
-      <c r="M3" s="3" t="s">
+      <c r="M3" s="3"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="N3" s="3" t="s">
+      <c r="B4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="O3" s="2"/>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
-        <v>2</v>
-      </c>
-      <c r="B4" s="4" t="s">
+      <c r="C4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="D4" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="E4" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="F4" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="G4" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="H4" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="I4" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="J4" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="K4" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="K4" s="5" t="s">
+      <c r="L4" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="L4" s="5" t="s">
+      <c r="M4" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="M4" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="N4" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="O4" s="5" t="s">
-        <v>30</v>
-      </c>
+      <c r="N4" s="2"/>
     </row>
   </sheetData>
   <autoFilter ref="A3:M3"/>
-  <mergeCells count="15">
-    <mergeCell ref="K1:O1"/>
+  <mergeCells count="13">
+    <mergeCell ref="H1:M1"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="B1:B3"/>
     <mergeCell ref="C1:C3"/>
@@ -666,13 +646,11 @@
     <mergeCell ref="E1:E3"/>
     <mergeCell ref="F1:F3"/>
     <mergeCell ref="G1:G3"/>
-    <mergeCell ref="H1:H3"/>
-    <mergeCell ref="I1:I3"/>
-    <mergeCell ref="J1:J3"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="I2:I3"/>
     <mergeCell ref="L2:L3"/>
-    <mergeCell ref="O2:O3"/>
+    <mergeCell ref="M2:M3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>